<commit_message>
Working 2.5 test cases
</commit_message>
<xml_diff>
--- a/error.xlsx
+++ b/error.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,932 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AK6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>typeCode</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>freqCode</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>refPeriodId</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>reporterCode</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>reporterDesc</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>reporterISO</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>flowCode</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>flowDesc</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>partnerCode</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>partnerDesc</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>partnerISO</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>partner2Code</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>partner2Desc</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>partner2ISO</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>classificationCode</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>cmdCode</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>cmdDesc</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>customsCode</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>customsDesc</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>mosCode</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>motCode</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>motDesc</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>qtyUnitCode</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>qtyUnitAbbr</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>qty</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>altQtyUnitCode</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>altQtyUnitAbbr</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>altQty</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>netWgt</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>grossWgt</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>cifvalue</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>fobvalue</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>primaryValue</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>CifValue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>20140101</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F2" t="n">
+        <v>579</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NOR</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>250</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Metropolitan France</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>FRA</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>H4</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>26011100</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="W2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Not available or not specified.</t>
+        </is>
+      </c>
+      <c r="Y2" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="AA2" t="n">
+        <v>6293</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>6293</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>1853.808528</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>1853.808528</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>1853.808528</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>6293</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1853.808528</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>20140101</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F3" t="n">
+        <v>579</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NOR</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>643</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Russian Federation</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>RUS</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>H4</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>26011100</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Not available or not specified.</t>
+        </is>
+      </c>
+      <c r="Y3" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="AA3" t="n">
+        <v>4949797</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>4949797</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>614197.868856</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>614197.868856</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>614197.868856</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>4949797</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>614197.868856</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>20140101</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F4" t="n">
+        <v>579</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NOR</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>442</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Luxembourg</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>LUX</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>H4</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>26011100</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="W4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Not available or not specified.</t>
+        </is>
+      </c>
+      <c r="Y4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="AA4" t="n">
+        <v>120000</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>120000</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>56043.59903999999</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>56043.59903999999</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>56043.59903999999</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>120000</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>56043.59903999999</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>20140101</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F5" t="n">
+        <v>579</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NOR</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>752</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>SWE</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>H4</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>26011100</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="W5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Not available or not specified.</t>
+        </is>
+      </c>
+      <c r="Y5" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="AA5" t="n">
+        <v>42818505</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>42818505</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>6420227.429616</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>6420227.429616</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>6420227.429616</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>44360168</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>6734740.564552</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>20140101</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F6" t="n">
+        <v>579</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NOR</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>826</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>GBR</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>H4</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>26011100</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="W6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Not available or not specified.</t>
+        </is>
+      </c>
+      <c r="Y6" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="AA6" t="n">
+        <v>8670</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>8670</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>2109.34724</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>2109.34724</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>2109.34724</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>8670</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>2109.34724</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>